<commit_message>
New sign in and sign up designs
</commit_message>
<xml_diff>
--- a/db/seeds_databases/vehicles_db.xlsx
+++ b/db/seeds_databases/vehicles_db.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27907"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/medularis/Library/Containers/com.microsoft.Excel/Data/Desktop/DesafioLatam/50-Parkwash/parkwash_rails_v2/db/seeds_databases/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/administrator/Desktop/Proyectos-Rails/parkwash/parkwash3/db/seeds_databases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBF63D9-1863-FE4E-BC66-E909FAF85AA6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{B9D82A25-DD8A-754E-BEFB-11D0168B5CFA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="109">
   <si>
     <t>DKZX-22</t>
   </si>
@@ -343,12 +348,21 @@
   </si>
   <si>
     <t>HD-1427</t>
+  </si>
+  <si>
+    <t>???_1</t>
+  </si>
+  <si>
+    <t>???_2</t>
+  </si>
+  <si>
+    <t>???_3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -739,11 +753,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B81763A-CF75-3F4D-AB76-3B313267E362}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1378,7 +1392,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>4</v>
+        <v>106</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>65</v>
@@ -1482,7 +1496,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>1</v>
@@ -1560,7 +1574,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>4</v>
+        <v>108</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>1</v>

</xml_diff>